<commit_message>
Optimize && Add examples
1. Optimize Framework
2. Support CC254x as MCU
3. Add three examples (APP_UART_Module, APP_RSSI_CHECK, APP_KEY)
</commit_message>
<xml_diff>
--- a/Instruction Table.xlsx
+++ b/Instruction Table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97">
   <si>
     <t>BLE Command</t>
   </si>
@@ -81,7 +81,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0x00: VERSION </t>
+      <t xml:space="preserve">0x00: INFO </t>
     </r>
     <r>
       <rPr>
@@ -91,7 +91,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">(Default: 0) </t>
+      <t xml:space="preserve">(Default: all 0x00) </t>
     </r>
     <r>
       <rPr>
@@ -101,53 +101,56 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(u32)</t>
+      <t>(bytes)</t>
+    </r>
+  </si>
+  <si>
+    <t>Value (Min: 0 byte, Max: 20 bytes)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x01: ENABLE_UPDATE_REQUEST </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Default: TRUE)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(bool)</t>
     </r>
   </si>
   <si>
     <t>Value (Min: 1 byte, Max: 4 bytes) (u8 - u32)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x01: ENABLE_UPDATE_REQUEST </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Default: TRUE)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(bool)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -716,7 +719,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Default: 16 0x00)</t>
+      <t>(Default: all 0x00)</t>
     </r>
     <r>
       <rPr>
@@ -736,7 +739,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(16 bytes)</t>
+      <t>(bytes)</t>
     </r>
   </si>
   <si>
@@ -792,6 +795,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">0x14: ENABLE_CMD_CHECK_BIT </t>
     </r>
     <r>
@@ -802,11 +812,300 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
+      <t>(Default: FALSE)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(bool)</t>
+    </r>
+  </si>
+  <si>
+    <t>0xFF: RESET</t>
+  </si>
+  <si>
+    <t>Any Value (Min: 1 byte, Max: 4 bytes) (u8 - u32)</t>
+  </si>
+  <si>
+    <t>0x05: Send Data</t>
+  </si>
+  <si>
+    <t>Related Devices Token (0 - 3)</t>
+  </si>
+  <si>
+    <t>Data (Min: 1 byte, Max: 20 bytes)</t>
+  </si>
+  <si>
+    <t>0x06: Reboot</t>
+  </si>
+  <si>
+    <t>0x07: Switch to Peripheral</t>
+  </si>
+  <si>
+    <t>0x08: Sleep (Sending Data via RX will wake device up and reboot device)</t>
+  </si>
+  <si>
+    <t>0x09: Set HAL</t>
+  </si>
+  <si>
+    <t>0x00: READ_RSSI_STATUS</t>
+  </si>
+  <si>
+    <t>Related Devices Token (0xFF)</t>
+  </si>
+  <si>
+    <t>0x70: Role Status Returned</t>
+  </si>
+  <si>
+    <t>Info (Min: 0 byte, Max: 20 bytes)</t>
+  </si>
+  <si>
+    <t>0x71: Connection Status Returned</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.25"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Device 0 Enable </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(bool)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.25"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Device 1 Enable </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(bool)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.25"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Device 2 Enable </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(bool)</t>
+    </r>
+  </si>
+  <si>
+    <t>0x72: Command is invalid</t>
+  </si>
+  <si>
+    <t>0x73: Set Parameters Successfully</t>
+  </si>
+  <si>
+    <t>0x74: Sended</t>
+  </si>
+  <si>
+    <t>Related Devices Token (0 - 2)</t>
+  </si>
+  <si>
+    <t>0x75: Unsend</t>
+  </si>
+  <si>
+    <t>0x76: Received</t>
+  </si>
+  <si>
+    <t>0x77: UnReceived</t>
+  </si>
+  <si>
+    <t>0x78: HAL Info Returned</t>
+  </si>
+  <si>
+    <t>0x01: Peripheral</t>
+  </si>
+  <si>
+    <t>0x00: Enable Advertisement</t>
+  </si>
+  <si>
+    <t>0x01: Disable Advertisement</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x01: ADVERTISING_INTERVAL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Default: 160)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(u16)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x02: ENABLE_DESIRED_REQUEST </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>(Default: TRUE)</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (bool)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x03: DESIRED_MIN_CONN_INTERVAL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Default: 32) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(u16)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x04: DESIRED_MAX_CONN_INTERVAL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Default: 32)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
         <charset val="134"/>
@@ -822,42 +1121,39 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(bool)</t>
-    </r>
-  </si>
-  <si>
-    <t>0xFF: RESET</t>
-  </si>
-  <si>
-    <t>Any Value (Min: 1 byte, Max: 4 bytes) (u8 - u32)</t>
-  </si>
-  <si>
-    <t>0x05: Send Data</t>
-  </si>
-  <si>
-    <t>Related Devices Token (0 - 3)</t>
-  </si>
-  <si>
-    <t>Data (Min: 1 byte, Max: 20 bytes)</t>
-  </si>
-  <si>
-    <t>0x06: Reboot</t>
-  </si>
-  <si>
-    <t>0x07: Switch to Peripheral</t>
-  </si>
-  <si>
-    <t>0x08: Sleep (Sending Data via RX will wake device up and reboot device)</t>
-  </si>
-  <si>
-    <t>0x09: Set HAL</t>
-  </si>
-  <si>
-    <t>0x00: READ_ADC_STATUS</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Channel + RESOLUTION </t>
+      <t>(u16)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x05: DESIRED_SLAVE_LATENCY </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Default: 0)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -867,19 +1163,19 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>[0x00 - 0x07: P0_0 - P0_7] + [0x00 + 0x30: 8\10\12\14]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x01: SET_LED_STATUS </t>
+      <t>(u8)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x06: DESIRED_CONN_TIMEOUT</t>
     </r>
     <r>
       <rPr>
@@ -889,7 +1185,39 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Default: FALSE)</t>
+      <t xml:space="preserve"> (Default: 200)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (u16)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0x07: CONN_PAUSE_PERIPHERAL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Default: 1)</t>
     </r>
     <r>
       <rPr>
@@ -909,155 +1237,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(bool)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pin [</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x00 - 0x0f: P0_0 - P1_7]</t>
-    </r>
-  </si>
-  <si>
-    <t>0x02: READ_KEY_STATUS</t>
-  </si>
-  <si>
-    <t>0x03: READ_RSSI_STATUS</t>
-  </si>
-  <si>
-    <t>Related Devices Token (0 - 2)</t>
-  </si>
-  <si>
-    <t>0x70: Role Status Returned</t>
-  </si>
-  <si>
-    <t>0x00: Sleep  0x01: Awake</t>
-  </si>
-  <si>
-    <t>Version(Min: 1 byte, Max: 4 bytes) (u8 - u32)</t>
-  </si>
-  <si>
-    <t>0x71: Connection Status Returned</t>
-  </si>
-  <si>
-    <t>Connected Devices Count (0 - 2)</t>
-  </si>
-  <si>
-    <t>Device 1 Token, Device 2 Token ...</t>
-  </si>
-  <si>
-    <t>0x72: Command is invalid</t>
-  </si>
-  <si>
-    <t>0x73: Set Parameters Successfully</t>
-  </si>
-  <si>
-    <t>0x74: Sended</t>
-  </si>
-  <si>
-    <t>0x75: Unsend</t>
-  </si>
-  <si>
-    <t>0x76: Received</t>
-  </si>
-  <si>
-    <t>0x77: UnReceived</t>
-  </si>
-  <si>
-    <t>0x78: HAL Info Returned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x01: SET_LED_STATUS </t>
-  </si>
-  <si>
-    <t>Value * (-1) (Min: 1 byte, Max: 4 bytes) (u8 - u32)</t>
-  </si>
-  <si>
-    <t>0x01: Peripheral</t>
-  </si>
-  <si>
-    <t>0x00: Enable Advertisement</t>
-  </si>
-  <si>
-    <t>0x01: Disable Advertisement</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x00: VERSION </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Default: 0) (u32)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x01: ADVERTISING_INTERVAL </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Default: 160)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>(u16)</t>
     </r>
   </si>
@@ -1070,221 +1249,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">0x02: ENABLE_DESIRED_REQUEST </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Default: TRUE)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (bool)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x03: DESIRED_MIN_CONN_INTERVAL </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(Default: 32) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(u16)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x04: DESIRED_MAX_CONN_INTERVAL </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Default: 32)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(u16)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x05: DESIRED_SLAVE_LATENCY </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Default: 0)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(u8)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0x06: DESIRED_CONN_TIMEOUT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Default: 200)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (u16)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">0x07: CONN_PAUSE_PERIPHERAL </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Default: 1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(u16)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>0x08: POWER_LEVEL</t>
     </r>
     <r>
@@ -1522,6 +1486,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">0x0e: SEND_DONE_DELAY </t>
     </r>
     <r>
@@ -1557,6 +1528,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">0x0f: ENABLE_TRANSMIT_ENCRYPT </t>
     </r>
     <r>
@@ -1613,6 +1591,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>0x10: TRANSMIT_ENCRYPT_KEY</t>
     </r>
     <r>
@@ -1623,7 +1608,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (Default: 16 0x00)</t>
+      <t xml:space="preserve"> (Default: all 0x00)</t>
     </r>
     <r>
       <rPr>
@@ -1643,11 +1628,18 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(16 bytes)</t>
-    </r>
-  </si>
-  <si>
-    <r>
+      <t>(bytes)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">0x11: WATCHDOG_MODE </t>
     </r>
     <r>
@@ -1689,6 +1681,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">0x12: ENABLE_CMD_CHECK_BIT </t>
     </r>
     <r>
@@ -1699,7 +1698,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(Default: TRUE)</t>
+      <t>(Default: FALSE)</t>
     </r>
     <r>
       <rPr>
@@ -1726,7 +1725,7 @@
     <t>0x05: Send Data (To central)</t>
   </si>
   <si>
-    <t>Related Devices Token (0xFF)</t>
+    <t>Related Devices Token (0x00)</t>
   </si>
   <si>
     <t>0x07: Switch to Central</t>
@@ -1735,10 +1734,7 @@
     <t>0x08: Sleep (PM3) (Sending Data via RX will wake device up and reboot device)</t>
   </si>
   <si>
-    <t>Connected Devices Count (0 - 1)</t>
-  </si>
-  <si>
-    <t>Device 1 Token(0xFF)...</t>
+    <t>Value * (-1) (Min: 1 byte, Max: 4 bytes) (u8 - u32)</t>
   </si>
 </sst>
 </file>
@@ -1746,8 +1742,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -1833,9 +1829,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1856,16 +1858,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1873,9 +1876,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1887,16 +1890,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1909,21 +1905,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -1939,25 +1928,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2037,19 +2033,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2067,19 +2135,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2091,31 +2159,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2127,67 +2177,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2203,24 +2217,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="47">
     <border>
@@ -2705,11 +2701,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2729,26 +2723,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2768,6 +2747,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2783,20 +2782,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2808,149 +2804,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="43" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3089,235 +3085,205 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3695,10 +3661,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B105"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3709,7 +3675,7 @@
     <col min="4" max="4" width="39.1238938053097" customWidth="1"/>
     <col min="5" max="5" width="59.2654867256637" customWidth="1"/>
     <col min="6" max="6" width="38.5752212389381" customWidth="1"/>
-    <col min="7" max="7" width="20.3893805309735" customWidth="1"/>
+    <col min="7" max="7" width="26.6371681415929" customWidth="1"/>
     <col min="8" max="8" width="33.3451327433628" customWidth="1"/>
     <col min="9" max="9" width="15.8053097345133" customWidth="1"/>
   </cols>
@@ -3733,11 +3699,11 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="88" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" ht="14.25" spans="1:9">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
         <v>6</v>
@@ -3754,7 +3720,7 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="101" t="s">
+      <c r="I2" s="89" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3773,7 +3739,7 @@
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="18"/>
-      <c r="I3" s="102" t="s">
+      <c r="I3" s="90" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3788,7 +3754,7 @@
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="18"/>
-      <c r="I4" s="103"/>
+      <c r="I4" s="91"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="7"/>
@@ -3801,7 +3767,7 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="103"/>
+      <c r="I5" s="91"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="7"/>
@@ -3814,7 +3780,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="18"/>
-      <c r="I6" s="103"/>
+      <c r="I6" s="91"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="7"/>
@@ -3831,7 +3797,7 @@
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
-      <c r="I7" s="103"/>
+      <c r="I7" s="91"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="7"/>
@@ -3842,11 +3808,11 @@
         <v>21</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
-      <c r="I8" s="103"/>
+      <c r="I8" s="91"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="7"/>
@@ -3854,14 +3820,14 @@
       <c r="C9" s="20"/>
       <c r="D9" s="24"/>
       <c r="E9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>22</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>20</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
-      <c r="I9" s="103"/>
+      <c r="I9" s="91"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="7"/>
@@ -3869,14 +3835,14 @@
       <c r="C10" s="20"/>
       <c r="D10" s="24"/>
       <c r="E10" s="22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
-      <c r="I10" s="103"/>
+      <c r="I10" s="91"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="7"/>
@@ -3884,14 +3850,14 @@
       <c r="C11" s="20"/>
       <c r="D11" s="24"/>
       <c r="E11" s="22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
-      <c r="I11" s="103"/>
+      <c r="I11" s="91"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="7"/>
@@ -3899,14 +3865,14 @@
       <c r="C12" s="20"/>
       <c r="D12" s="24"/>
       <c r="E12" s="22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
-      <c r="I12" s="103"/>
+      <c r="I12" s="91"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7"/>
@@ -3914,14 +3880,14 @@
       <c r="C13" s="20"/>
       <c r="D13" s="24"/>
       <c r="E13" s="22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
-      <c r="I13" s="103"/>
+      <c r="I13" s="91"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7"/>
@@ -3929,16 +3895,16 @@
       <c r="C14" s="20"/>
       <c r="D14" s="24"/>
       <c r="E14" s="22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H14" s="23"/>
-      <c r="I14" s="103"/>
+      <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="7"/>
@@ -3946,14 +3912,14 @@
       <c r="C15" s="20"/>
       <c r="D15" s="24"/>
       <c r="E15" s="22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
-      <c r="I15" s="103"/>
+      <c r="I15" s="91"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="7"/>
@@ -3961,14 +3927,14 @@
       <c r="C16" s="20"/>
       <c r="D16" s="24"/>
       <c r="E16" s="22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
-      <c r="I16" s="103"/>
+      <c r="I16" s="91"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="7"/>
@@ -3976,14 +3942,14 @@
       <c r="C17" s="20"/>
       <c r="D17" s="24"/>
       <c r="E17" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
-      <c r="I17" s="103"/>
+      <c r="I17" s="91"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="7"/>
@@ -3991,14 +3957,14 @@
       <c r="C18" s="20"/>
       <c r="D18" s="24"/>
       <c r="E18" s="22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
-      <c r="I18" s="103"/>
+      <c r="I18" s="91"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="7"/>
@@ -4006,14 +3972,14 @@
       <c r="C19" s="20"/>
       <c r="D19" s="24"/>
       <c r="E19" s="22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
-      <c r="I19" s="103"/>
+      <c r="I19" s="91"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="7"/>
@@ -4021,14 +3987,14 @@
       <c r="C20" s="20"/>
       <c r="D20" s="24"/>
       <c r="E20" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
-      <c r="I20" s="103"/>
+      <c r="I20" s="91"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="7"/>
@@ -4036,14 +4002,14 @@
       <c r="C21" s="20"/>
       <c r="D21" s="24"/>
       <c r="E21" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
-      <c r="I21" s="103"/>
+      <c r="I21" s="91"/>
     </row>
     <row r="22" ht="94.5" spans="1:9">
       <c r="A22" s="7"/>
@@ -4051,14 +4017,14 @@
       <c r="C22" s="20"/>
       <c r="D22" s="24"/>
       <c r="E22" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
-      <c r="I22" s="103"/>
+      <c r="I22" s="91"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="7"/>
@@ -4066,14 +4032,14 @@
       <c r="C23" s="20"/>
       <c r="D23" s="24"/>
       <c r="E23" s="22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
-      <c r="I23" s="103"/>
+      <c r="I23" s="91"/>
     </row>
     <row r="24" ht="27" spans="1:9">
       <c r="A24" s="7"/>
@@ -4081,14 +4047,14 @@
       <c r="C24" s="20"/>
       <c r="D24" s="24"/>
       <c r="E24" s="22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
-      <c r="I24" s="103"/>
+      <c r="I24" s="91"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="7"/>
@@ -4096,14 +4062,14 @@
       <c r="C25" s="20"/>
       <c r="D25" s="24"/>
       <c r="E25" s="22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G25" s="27"/>
       <c r="H25" s="28"/>
-      <c r="I25" s="103"/>
+      <c r="I25" s="91"/>
     </row>
     <row r="26" ht="94.5" spans="1:9">
       <c r="A26" s="7"/>
@@ -4111,14 +4077,14 @@
       <c r="C26" s="20"/>
       <c r="D26" s="24"/>
       <c r="E26" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G26" s="23"/>
       <c r="H26" s="23"/>
-      <c r="I26" s="103"/>
+      <c r="I26" s="91"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="7"/>
@@ -4126,14 +4092,14 @@
       <c r="C27" s="20"/>
       <c r="D27" s="24"/>
       <c r="E27" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
-      <c r="I27" s="103"/>
+      <c r="I27" s="91"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="7"/>
@@ -4141,14 +4107,14 @@
       <c r="C28" s="20"/>
       <c r="D28" s="24"/>
       <c r="E28" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>
-      <c r="I28" s="103"/>
+      <c r="I28" s="91"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="7"/>
@@ -4159,7 +4125,7 @@
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
       <c r="H29" s="32"/>
-      <c r="I29" s="103"/>
+      <c r="I29" s="91"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="7"/>
@@ -4170,420 +4136,386 @@
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
       <c r="H30" s="32"/>
-      <c r="I30" s="103"/>
+      <c r="I30" s="91"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="7"/>
       <c r="B31" s="19"/>
       <c r="C31" s="20"/>
       <c r="D31" s="34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E31" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F31" s="36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G31" s="37"/>
       <c r="H31" s="38"/>
-      <c r="I31" s="103"/>
+      <c r="I31" s="91"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="7"/>
       <c r="B32" s="19"/>
       <c r="C32" s="20"/>
       <c r="D32" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E32" s="16"/>
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
       <c r="H32" s="18"/>
-      <c r="I32" s="103"/>
+      <c r="I32" s="91"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="7"/>
       <c r="B33" s="19"/>
       <c r="C33" s="39"/>
       <c r="D33" s="40" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E33" s="16"/>
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
       <c r="H33" s="18"/>
-      <c r="I33" s="103"/>
+      <c r="I33" s="91"/>
     </row>
     <row r="34" ht="27" spans="1:9">
       <c r="A34" s="7"/>
       <c r="B34" s="19"/>
       <c r="C34" s="39"/>
       <c r="D34" s="41" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E34" s="42"/>
       <c r="F34" s="43"/>
       <c r="G34" s="43"/>
       <c r="H34" s="44"/>
-      <c r="I34" s="103"/>
-    </row>
-    <row r="35" ht="40.5" spans="1:9">
+      <c r="I34" s="91"/>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="7"/>
       <c r="B35" s="19"/>
       <c r="C35" s="20"/>
       <c r="D35" s="45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="F35" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="103"/>
+      <c r="F35" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="91"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="7"/>
       <c r="B36" s="19"/>
       <c r="C36" s="20"/>
       <c r="D36" s="45"/>
-      <c r="E36" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="G36" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="52"/>
-      <c r="I36" s="103"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="91"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="7"/>
       <c r="B37" s="19"/>
       <c r="C37" s="20"/>
       <c r="D37" s="45"/>
-      <c r="E37" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="F37" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="G37" s="53"/>
-      <c r="H37" s="54"/>
-      <c r="I37" s="103"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="91"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="7"/>
       <c r="B38" s="19"/>
       <c r="C38" s="20"/>
       <c r="D38" s="45"/>
-      <c r="E38" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="F38" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="G38" s="53"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="103"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="91"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="7"/>
       <c r="B39" s="19"/>
       <c r="C39" s="39"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="57"/>
-      <c r="I39" s="103"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="91"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="7"/>
       <c r="B40" s="19"/>
       <c r="C40" s="39"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="59"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="103"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="91"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="7"/>
       <c r="B41" s="19"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E41" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="G41" s="64"/>
-      <c r="H41" s="65"/>
-      <c r="I41" s="103"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="59"/>
+      <c r="G41" s="59"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="91"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="7"/>
       <c r="B42" s="19"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" s="68" t="s">
-        <v>65</v>
-      </c>
-      <c r="F42" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="G42" s="70"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="103"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="H42" s="64"/>
+      <c r="I42" s="91"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="7"/>
       <c r="B43" s="19"/>
       <c r="C43" s="20"/>
-      <c r="D43" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="73"/>
-      <c r="F43" s="74"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="75"/>
-      <c r="I43" s="103"/>
+      <c r="D43" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="66"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="91"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="7"/>
       <c r="B44" s="19"/>
       <c r="C44" s="20"/>
-      <c r="D44" s="72" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="73"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="75"/>
-      <c r="I44" s="103"/>
+      <c r="D44" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="66"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="68"/>
+      <c r="I44" s="91"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="7"/>
       <c r="B45" s="19"/>
       <c r="C45" s="20"/>
-      <c r="D45" s="67" t="s">
-        <v>69</v>
+      <c r="D45" s="62" t="s">
+        <v>65</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" s="73"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="75"/>
-      <c r="I45" s="103"/>
+        <v>66</v>
+      </c>
+      <c r="F45" s="66"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="91"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="7"/>
       <c r="B46" s="19"/>
       <c r="C46" s="39"/>
-      <c r="D46" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="F46" s="73"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="75"/>
-      <c r="I46" s="103"/>
+      <c r="D46" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="F46" s="66"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="68"/>
+      <c r="I46" s="91"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="7"/>
       <c r="B47" s="19"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="E47" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="F47" s="80" t="s">
-        <v>49</v>
-      </c>
-      <c r="G47" s="81"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="103"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="E47" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="73"/>
+      <c r="H47" s="74"/>
+      <c r="I47" s="91"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="7"/>
       <c r="B48" s="19"/>
-      <c r="C48" s="78"/>
-      <c r="D48" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="E48" s="79" t="s">
-        <v>60</v>
-      </c>
-      <c r="F48" s="83"/>
-      <c r="G48" s="83"/>
-      <c r="H48" s="83"/>
-      <c r="I48" s="103"/>
-    </row>
-    <row r="49" ht="40.5" spans="1:9">
+      <c r="C48" s="71"/>
+      <c r="D48" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="91"/>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="7"/>
       <c r="B49" s="19"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="84" t="s">
-        <v>73</v>
+      <c r="C49" s="71"/>
+      <c r="D49" s="75" t="s">
+        <v>70</v>
       </c>
       <c r="E49" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="F49" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="G49" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H49" s="52"/>
-      <c r="I49" s="103"/>
+      <c r="F49" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="91"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="7"/>
       <c r="B50" s="19"/>
-      <c r="C50" s="78"/>
-      <c r="D50" s="84"/>
-      <c r="E50" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="F50" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="G50" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H50" s="52"/>
-      <c r="I50" s="103"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="75"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="91"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="7"/>
       <c r="B51" s="19"/>
-      <c r="C51" s="78"/>
-      <c r="D51" s="84"/>
-      <c r="E51" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="F51" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="G51" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H51" s="52"/>
-      <c r="I51" s="103"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="75"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="91"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="7"/>
       <c r="B52" s="19"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="84"/>
-      <c r="E52" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="F52" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="G52" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="H52" s="52"/>
-      <c r="I52" s="103"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="75"/>
+      <c r="E52" s="48"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="91"/>
     </row>
     <row r="53" ht="14.25" spans="1:9">
       <c r="A53" s="7"/>
       <c r="B53" s="19"/>
-      <c r="C53" s="85"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
-      <c r="H53" s="87"/>
-      <c r="I53" s="103"/>
+      <c r="C53" s="76"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="77"/>
+      <c r="F53" s="77"/>
+      <c r="G53" s="77"/>
+      <c r="H53" s="78"/>
+      <c r="I53" s="91"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="7"/>
       <c r="B54" s="19"/>
-      <c r="C54" s="88"/>
-      <c r="D54" s="88"/>
-      <c r="E54" s="88"/>
-      <c r="F54" s="88"/>
-      <c r="G54" s="88"/>
-      <c r="H54" s="88"/>
-      <c r="I54" s="104"/>
+      <c r="C54" s="79"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="79"/>
+      <c r="F54" s="79"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="92"/>
     </row>
     <row r="55" ht="14.25" spans="1:9">
       <c r="A55" s="7"/>
       <c r="B55" s="19"/>
-      <c r="C55" s="88"/>
-      <c r="D55" s="88"/>
-      <c r="E55" s="88"/>
-      <c r="F55" s="88"/>
-      <c r="G55" s="88"/>
-      <c r="H55" s="88"/>
-      <c r="I55" s="104"/>
+      <c r="C55" s="79"/>
+      <c r="D55" s="79"/>
+      <c r="E55" s="79"/>
+      <c r="F55" s="79"/>
+      <c r="G55" s="79"/>
+      <c r="H55" s="79"/>
+      <c r="I55" s="92"/>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="7"/>
       <c r="B56" s="19"/>
-      <c r="C56" s="89" t="s">
-        <v>76</v>
-      </c>
-      <c r="D56" s="90" t="s">
-        <v>77</v>
+      <c r="C56" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="81" t="s">
+        <v>72</v>
       </c>
       <c r="E56" s="16"/>
       <c r="F56" s="17"/>
       <c r="G56" s="17"/>
       <c r="H56" s="18"/>
-      <c r="I56" s="103"/>
+      <c r="I56" s="91"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="91"/>
+      <c r="A57" s="82"/>
       <c r="B57" s="19"/>
-      <c r="C57" s="92"/>
+      <c r="C57" s="83"/>
       <c r="D57" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" s="93"/>
-      <c r="F57" s="94"/>
-      <c r="G57" s="94"/>
-      <c r="H57" s="95"/>
-      <c r="I57" s="103"/>
+        <v>73</v>
+      </c>
+      <c r="E57" s="48"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="91"/>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="91"/>
+      <c r="A58" s="82"/>
       <c r="B58" s="19"/>
-      <c r="C58" s="92"/>
+      <c r="C58" s="83"/>
       <c r="D58" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="93"/>
-      <c r="F58" s="94"/>
-      <c r="G58" s="94"/>
-      <c r="H58" s="95"/>
-      <c r="I58" s="103"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="50"/>
+      <c r="I58" s="91"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="7"/>
       <c r="B59" s="19"/>
-      <c r="C59" s="96"/>
+      <c r="C59" s="84"/>
       <c r="D59" s="34" t="s">
         <v>17</v>
       </c>
@@ -4591,690 +4523,676 @@
       <c r="F59" s="17"/>
       <c r="G59" s="17"/>
       <c r="H59" s="18"/>
-      <c r="I59" s="103"/>
+      <c r="I59" s="91"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="7"/>
       <c r="B60" s="19"/>
-      <c r="C60" s="97"/>
-      <c r="D60" s="98" t="s">
+      <c r="C60" s="85"/>
+      <c r="D60" s="86" t="s">
         <v>18</v>
       </c>
       <c r="E60" s="22" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="F60" s="23" t="s">
         <v>20</v>
       </c>
       <c r="G60" s="23"/>
       <c r="H60" s="23"/>
-      <c r="I60" s="103"/>
+      <c r="I60" s="91"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="7"/>
       <c r="B61" s="19"/>
-      <c r="C61" s="97"/>
-      <c r="D61" s="99"/>
-      <c r="E61" s="49" t="s">
-        <v>80</v>
+      <c r="C61" s="85"/>
+      <c r="D61" s="87"/>
+      <c r="E61" s="46" t="s">
+        <v>74</v>
       </c>
       <c r="F61" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G61" s="23"/>
       <c r="H61" s="23"/>
-      <c r="I61" s="103"/>
+      <c r="I61" s="91"/>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="7"/>
       <c r="B62" s="19"/>
-      <c r="C62" s="97"/>
-      <c r="D62" s="99"/>
-      <c r="E62" s="49" t="s">
-        <v>81</v>
+      <c r="C62" s="85"/>
+      <c r="D62" s="87"/>
+      <c r="E62" s="46" t="s">
+        <v>75</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G62" s="23"/>
       <c r="H62" s="23"/>
-      <c r="I62" s="103"/>
+      <c r="I62" s="91"/>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" s="7"/>
       <c r="B63" s="19"/>
-      <c r="C63" s="97"/>
-      <c r="D63" s="99"/>
-      <c r="E63" s="49" t="s">
-        <v>82</v>
+      <c r="C63" s="85"/>
+      <c r="D63" s="87"/>
+      <c r="E63" s="46" t="s">
+        <v>76</v>
       </c>
       <c r="F63" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G63" s="23"/>
       <c r="H63" s="23"/>
-      <c r="I63" s="103"/>
+      <c r="I63" s="91"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="7"/>
       <c r="B64" s="19"/>
-      <c r="C64" s="97"/>
-      <c r="D64" s="99"/>
-      <c r="E64" s="49" t="s">
-        <v>83</v>
+      <c r="C64" s="85"/>
+      <c r="D64" s="87"/>
+      <c r="E64" s="46" t="s">
+        <v>77</v>
       </c>
       <c r="F64" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G64" s="23"/>
       <c r="H64" s="23"/>
-      <c r="I64" s="103"/>
+      <c r="I64" s="91"/>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="7"/>
       <c r="B65" s="19"/>
-      <c r="C65" s="97"/>
-      <c r="D65" s="99"/>
-      <c r="E65" s="49" t="s">
-        <v>84</v>
+      <c r="C65" s="85"/>
+      <c r="D65" s="87"/>
+      <c r="E65" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G65" s="23"/>
       <c r="H65" s="23"/>
-      <c r="I65" s="103"/>
+      <c r="I65" s="91"/>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="7"/>
       <c r="B66" s="19"/>
-      <c r="C66" s="97"/>
-      <c r="D66" s="99"/>
-      <c r="E66" s="49" t="s">
-        <v>85</v>
+      <c r="C66" s="85"/>
+      <c r="D66" s="87"/>
+      <c r="E66" s="46" t="s">
+        <v>79</v>
       </c>
       <c r="F66" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G66" s="23"/>
       <c r="H66" s="23"/>
-      <c r="I66" s="103"/>
+      <c r="I66" s="91"/>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="7"/>
       <c r="B67" s="19"/>
-      <c r="C67" s="97"/>
-      <c r="D67" s="99"/>
-      <c r="E67" s="49" t="s">
-        <v>86</v>
+      <c r="C67" s="85"/>
+      <c r="D67" s="87"/>
+      <c r="E67" s="46" t="s">
+        <v>80</v>
       </c>
       <c r="F67" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G67" s="23"/>
       <c r="H67" s="23"/>
-      <c r="I67" s="103"/>
+      <c r="I67" s="91"/>
     </row>
     <row r="68" ht="94.5" spans="1:9">
       <c r="A68" s="7"/>
       <c r="B68" s="19"/>
-      <c r="C68" s="97"/>
-      <c r="D68" s="99"/>
-      <c r="E68" s="50" t="s">
-        <v>87</v>
+      <c r="C68" s="85"/>
+      <c r="D68" s="87"/>
+      <c r="E68" s="93" t="s">
+        <v>81</v>
       </c>
       <c r="F68" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G68" s="23"/>
       <c r="H68" s="23"/>
-      <c r="I68" s="103"/>
+      <c r="I68" s="91"/>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="7"/>
       <c r="B69" s="19"/>
-      <c r="C69" s="97"/>
-      <c r="D69" s="99"/>
-      <c r="E69" s="49" t="s">
-        <v>88</v>
+      <c r="C69" s="85"/>
+      <c r="D69" s="87"/>
+      <c r="E69" s="46" t="s">
+        <v>82</v>
       </c>
       <c r="F69" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G69" s="23"/>
       <c r="H69" s="23"/>
-      <c r="I69" s="103"/>
+      <c r="I69" s="91"/>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="7"/>
       <c r="B70" s="19"/>
-      <c r="C70" s="97"/>
-      <c r="D70" s="99"/>
-      <c r="E70" s="49" t="s">
-        <v>89</v>
+      <c r="C70" s="85"/>
+      <c r="D70" s="87"/>
+      <c r="E70" s="46" t="s">
+        <v>83</v>
       </c>
       <c r="F70" s="23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G70" s="23"/>
       <c r="H70" s="23"/>
-      <c r="I70" s="103"/>
+      <c r="I70" s="91"/>
     </row>
     <row r="71" ht="94.5" spans="1:9">
       <c r="A71" s="7"/>
       <c r="B71" s="19"/>
-      <c r="C71" s="97"/>
-      <c r="D71" s="99"/>
-      <c r="E71" s="50" t="s">
-        <v>90</v>
+      <c r="C71" s="85"/>
+      <c r="D71" s="87"/>
+      <c r="E71" s="93" t="s">
+        <v>84</v>
       </c>
       <c r="F71" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G71" s="23"/>
       <c r="H71" s="23"/>
-      <c r="I71" s="103"/>
+      <c r="I71" s="91"/>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="7"/>
       <c r="B72" s="19"/>
-      <c r="C72" s="97"/>
-      <c r="D72" s="99"/>
-      <c r="E72" s="49" t="s">
-        <v>91</v>
+      <c r="C72" s="85"/>
+      <c r="D72" s="87"/>
+      <c r="E72" s="46" t="s">
+        <v>85</v>
       </c>
       <c r="F72" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G72" s="23"/>
       <c r="H72" s="23"/>
-      <c r="I72" s="103"/>
+      <c r="I72" s="91"/>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="7"/>
       <c r="B73" s="19"/>
-      <c r="C73" s="97"/>
-      <c r="D73" s="99"/>
-      <c r="E73" s="49" t="s">
-        <v>92</v>
+      <c r="C73" s="85"/>
+      <c r="D73" s="87"/>
+      <c r="E73" s="46" t="s">
+        <v>86</v>
       </c>
       <c r="F73" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G73" s="23"/>
       <c r="H73" s="23"/>
-      <c r="I73" s="103"/>
+      <c r="I73" s="91"/>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="7"/>
       <c r="B74" s="19"/>
-      <c r="C74" s="97"/>
-      <c r="D74" s="99"/>
-      <c r="E74" s="49" t="s">
-        <v>93</v>
+      <c r="C74" s="85"/>
+      <c r="D74" s="87"/>
+      <c r="E74" s="46" t="s">
+        <v>87</v>
       </c>
       <c r="F74" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G74" s="23"/>
       <c r="H74" s="23"/>
-      <c r="I74" s="103"/>
+      <c r="I74" s="91"/>
     </row>
     <row r="75" ht="27" spans="1:9">
       <c r="A75" s="7"/>
       <c r="B75" s="19"/>
-      <c r="C75" s="97"/>
-      <c r="D75" s="99"/>
+      <c r="C75" s="85"/>
+      <c r="D75" s="87"/>
       <c r="E75" s="22" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F75" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G75" s="23"/>
       <c r="H75" s="23"/>
-      <c r="I75" s="103"/>
+      <c r="I75" s="91"/>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="7"/>
       <c r="B76" s="19"/>
-      <c r="C76" s="97"/>
-      <c r="D76" s="99"/>
+      <c r="C76" s="85"/>
+      <c r="D76" s="87"/>
       <c r="E76" s="22" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F76" s="26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G76" s="27"/>
       <c r="H76" s="28"/>
-      <c r="I76" s="103"/>
+      <c r="I76" s="91"/>
     </row>
     <row r="77" ht="94.5" spans="1:9">
       <c r="A77" s="7"/>
       <c r="B77" s="19"/>
-      <c r="C77" s="97"/>
-      <c r="D77" s="99"/>
+      <c r="C77" s="85"/>
+      <c r="D77" s="87"/>
       <c r="E77" s="22" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F77" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G77" s="23"/>
       <c r="H77" s="23"/>
-      <c r="I77" s="103"/>
+      <c r="I77" s="91"/>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="7"/>
       <c r="B78" s="19"/>
-      <c r="C78" s="97"/>
-      <c r="D78" s="99"/>
+      <c r="C78" s="85"/>
+      <c r="D78" s="87"/>
       <c r="E78" s="22" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F78" s="23" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G78" s="23"/>
       <c r="H78" s="23"/>
-      <c r="I78" s="103"/>
+      <c r="I78" s="91"/>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" s="7"/>
       <c r="B79" s="19"/>
-      <c r="C79" s="97"/>
-      <c r="D79" s="99"/>
-      <c r="E79" s="105" t="s">
-        <v>45</v>
+      <c r="C79" s="85"/>
+      <c r="D79" s="87"/>
+      <c r="E79" s="94" t="s">
+        <v>46</v>
       </c>
       <c r="F79" s="23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G79" s="23"/>
       <c r="H79" s="23"/>
-      <c r="I79" s="103"/>
+      <c r="I79" s="91"/>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="7"/>
       <c r="B80" s="19"/>
-      <c r="C80" s="97"/>
-      <c r="D80" s="99"/>
-      <c r="E80" s="83"/>
-      <c r="F80" s="83"/>
-      <c r="G80" s="83"/>
-      <c r="H80" s="83"/>
-      <c r="I80" s="103"/>
+      <c r="C80" s="85"/>
+      <c r="D80" s="87"/>
+      <c r="E80" s="64"/>
+      <c r="F80" s="64"/>
+      <c r="G80" s="64"/>
+      <c r="H80" s="64"/>
+      <c r="I80" s="91"/>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="7"/>
       <c r="B81" s="19"/>
-      <c r="C81" s="97"/>
-      <c r="D81" s="106"/>
-      <c r="E81" s="83"/>
-      <c r="F81" s="83"/>
-      <c r="G81" s="83"/>
-      <c r="H81" s="83"/>
-      <c r="I81" s="103"/>
+      <c r="C81" s="85"/>
+      <c r="D81" s="95"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="64"/>
+      <c r="G81" s="64"/>
+      <c r="H81" s="64"/>
+      <c r="I81" s="91"/>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="7"/>
       <c r="B82" s="19"/>
-      <c r="C82" s="97"/>
+      <c r="C82" s="85"/>
       <c r="D82" s="34" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E82" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="F82" s="107" t="s">
-        <v>49</v>
-      </c>
-      <c r="G82" s="108"/>
-      <c r="H82" s="109"/>
-      <c r="I82" s="103"/>
+        <v>93</v>
+      </c>
+      <c r="F82" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="G82" s="97"/>
+      <c r="H82" s="98"/>
+      <c r="I82" s="91"/>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="7"/>
       <c r="B83" s="19"/>
-      <c r="C83" s="97"/>
+      <c r="C83" s="85"/>
       <c r="D83" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="E83" s="110"/>
-      <c r="F83" s="111"/>
-      <c r="G83" s="111"/>
-      <c r="H83" s="112"/>
-      <c r="I83" s="103"/>
+        <v>51</v>
+      </c>
+      <c r="E83" s="99"/>
+      <c r="F83" s="100"/>
+      <c r="G83" s="100"/>
+      <c r="H83" s="101"/>
+      <c r="I83" s="91"/>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="7"/>
       <c r="B84" s="19"/>
-      <c r="C84" s="97"/>
-      <c r="D84" s="113" t="s">
-        <v>100</v>
-      </c>
-      <c r="E84" s="110"/>
-      <c r="F84" s="111"/>
-      <c r="G84" s="111"/>
-      <c r="H84" s="112"/>
-      <c r="I84" s="103"/>
+      <c r="C84" s="85"/>
+      <c r="D84" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="E84" s="99"/>
+      <c r="F84" s="100"/>
+      <c r="G84" s="100"/>
+      <c r="H84" s="101"/>
+      <c r="I84" s="91"/>
     </row>
     <row r="85" ht="27" spans="1:9">
       <c r="A85" s="7"/>
       <c r="B85" s="19"/>
-      <c r="C85" s="114"/>
+      <c r="C85" s="103"/>
       <c r="D85" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="E85" s="83"/>
-      <c r="F85" s="83"/>
-      <c r="G85" s="83"/>
-      <c r="H85" s="83"/>
-      <c r="I85" s="103"/>
-    </row>
-    <row r="86" ht="40.5" spans="1:9">
+        <v>95</v>
+      </c>
+      <c r="E85" s="64"/>
+      <c r="F85" s="64"/>
+      <c r="G85" s="64"/>
+      <c r="H85" s="64"/>
+      <c r="I85" s="91"/>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86" s="7"/>
       <c r="B86" s="19"/>
-      <c r="C86" s="114"/>
-      <c r="D86" s="115" t="s">
-        <v>53</v>
+      <c r="C86" s="103"/>
+      <c r="D86" s="104" t="s">
+        <v>54</v>
       </c>
       <c r="E86" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="F86" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="G86" s="48"/>
-      <c r="H86" s="48"/>
-      <c r="I86" s="103"/>
+      <c r="F86" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="G86" s="47"/>
+      <c r="H86" s="47"/>
+      <c r="I86" s="91"/>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="7"/>
       <c r="B87" s="19"/>
-      <c r="C87" s="114"/>
-      <c r="D87" s="115"/>
-      <c r="E87" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="F87" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="G87" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H87" s="52"/>
-      <c r="I87" s="103"/>
+      <c r="C87" s="103"/>
+      <c r="D87" s="104"/>
+      <c r="E87" s="48"/>
+      <c r="F87" s="49"/>
+      <c r="G87" s="49"/>
+      <c r="H87" s="50"/>
+      <c r="I87" s="91"/>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="7"/>
       <c r="B88" s="19"/>
-      <c r="C88" s="114"/>
-      <c r="D88" s="115"/>
-      <c r="E88" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="F88" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="G88" s="53"/>
-      <c r="H88" s="54"/>
-      <c r="I88" s="103"/>
+      <c r="C88" s="103"/>
+      <c r="D88" s="104"/>
+      <c r="E88" s="48"/>
+      <c r="F88" s="49"/>
+      <c r="G88" s="49"/>
+      <c r="H88" s="50"/>
+      <c r="I88" s="91"/>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="7"/>
       <c r="B89" s="19"/>
-      <c r="C89" s="114"/>
-      <c r="D89" s="115"/>
-      <c r="E89" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="F89" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="G89" s="53"/>
-      <c r="H89" s="54"/>
-      <c r="I89" s="103"/>
+      <c r="C89" s="103"/>
+      <c r="D89" s="104"/>
+      <c r="E89" s="48"/>
+      <c r="F89" s="49"/>
+      <c r="G89" s="49"/>
+      <c r="H89" s="50"/>
+      <c r="I89" s="91"/>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="7"/>
       <c r="B90" s="19"/>
-      <c r="C90" s="114"/>
-      <c r="D90" s="55"/>
-      <c r="E90" s="83"/>
-      <c r="F90" s="83"/>
-      <c r="G90" s="83"/>
-      <c r="H90" s="83"/>
-      <c r="I90" s="103"/>
+      <c r="C90" s="103"/>
+      <c r="D90" s="51"/>
+      <c r="E90" s="64"/>
+      <c r="F90" s="64"/>
+      <c r="G90" s="64"/>
+      <c r="H90" s="64"/>
+      <c r="I90" s="91"/>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="7"/>
       <c r="B91" s="19"/>
-      <c r="C91" s="114"/>
-      <c r="D91" s="58"/>
-      <c r="E91" s="116"/>
-      <c r="F91" s="117"/>
-      <c r="G91" s="117"/>
-      <c r="H91" s="117"/>
-      <c r="I91" s="103"/>
+      <c r="C91" s="103"/>
+      <c r="D91" s="54"/>
+      <c r="E91" s="105"/>
+      <c r="F91" s="106"/>
+      <c r="G91" s="106"/>
+      <c r="H91" s="106"/>
+      <c r="I91" s="91"/>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="7"/>
       <c r="B92" s="19"/>
-      <c r="C92" s="97"/>
-      <c r="D92" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E92" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="F92" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="G92" s="64"/>
-      <c r="H92" s="65"/>
-      <c r="I92" s="103"/>
+      <c r="C92" s="85"/>
+      <c r="D92" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E92" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="F92" s="59"/>
+      <c r="G92" s="59"/>
+      <c r="H92" s="60"/>
+      <c r="I92" s="91"/>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="7"/>
       <c r="B93" s="19"/>
-      <c r="C93" s="97"/>
-      <c r="D93" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="E93" s="79" t="s">
-        <v>102</v>
-      </c>
-      <c r="F93" s="118" t="s">
-        <v>103</v>
-      </c>
-      <c r="G93" s="118"/>
-      <c r="H93" s="118"/>
-      <c r="I93" s="103"/>
+      <c r="C93" s="85"/>
+      <c r="D93" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="E93" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="F93" s="55"/>
+      <c r="G93" s="55"/>
+      <c r="H93" s="55"/>
+      <c r="I93" s="91"/>
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="7"/>
       <c r="B94" s="19"/>
-      <c r="C94" s="97"/>
-      <c r="D94" s="67" t="s">
-        <v>67</v>
-      </c>
-      <c r="E94" s="59"/>
-      <c r="F94" s="59"/>
-      <c r="G94" s="59"/>
-      <c r="H94" s="60"/>
-      <c r="I94" s="103"/>
+      <c r="C94" s="85"/>
+      <c r="D94" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="E94" s="55"/>
+      <c r="F94" s="55"/>
+      <c r="G94" s="55"/>
+      <c r="H94" s="56"/>
+      <c r="I94" s="91"/>
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="7"/>
       <c r="B95" s="19"/>
-      <c r="C95" s="97"/>
-      <c r="D95" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="E95" s="59"/>
-      <c r="F95" s="59"/>
-      <c r="G95" s="59"/>
-      <c r="H95" s="60"/>
-      <c r="I95" s="103"/>
+      <c r="C95" s="85"/>
+      <c r="D95" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="E95" s="55"/>
+      <c r="F95" s="55"/>
+      <c r="G95" s="55"/>
+      <c r="H95" s="56"/>
+      <c r="I95" s="91"/>
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="7"/>
       <c r="B96" s="19"/>
-      <c r="C96" s="97"/>
-      <c r="D96" s="67" t="s">
-        <v>69</v>
-      </c>
-      <c r="E96" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="F96" s="119"/>
-      <c r="G96" s="119"/>
-      <c r="H96" s="120"/>
-      <c r="I96" s="103"/>
+      <c r="C96" s="85"/>
+      <c r="D96" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="E96" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F96" s="107"/>
+      <c r="G96" s="107"/>
+      <c r="H96" s="108"/>
+      <c r="I96" s="91"/>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="7"/>
       <c r="B97" s="19"/>
-      <c r="C97" s="97"/>
-      <c r="D97" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="E97" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="F97" s="119"/>
-      <c r="G97" s="119"/>
-      <c r="H97" s="120"/>
-      <c r="I97" s="103"/>
+      <c r="C97" s="85"/>
+      <c r="D97" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="E97" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F97" s="107"/>
+      <c r="G97" s="107"/>
+      <c r="H97" s="108"/>
+      <c r="I97" s="91"/>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="7"/>
       <c r="B98" s="19"/>
-      <c r="C98" s="97"/>
-      <c r="D98" s="67" t="s">
-        <v>71</v>
-      </c>
-      <c r="E98" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="F98" s="121" t="s">
-        <v>49</v>
-      </c>
-      <c r="G98" s="81"/>
-      <c r="H98" s="82"/>
-      <c r="I98" s="103"/>
+      <c r="C98" s="85"/>
+      <c r="D98" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="E98" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F98" s="109" t="s">
+        <v>50</v>
+      </c>
+      <c r="G98" s="73"/>
+      <c r="H98" s="74"/>
+      <c r="I98" s="91"/>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="7"/>
       <c r="B99" s="19"/>
-      <c r="C99" s="97"/>
-      <c r="D99" s="67" t="s">
-        <v>72</v>
-      </c>
-      <c r="E99" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="F99" s="83"/>
-      <c r="G99" s="83"/>
-      <c r="H99" s="83"/>
-      <c r="I99" s="103"/>
-    </row>
-    <row r="100" ht="40.5" spans="1:9">
+      <c r="C99" s="85"/>
+      <c r="D99" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="E99" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="F99" s="64"/>
+      <c r="G99" s="64"/>
+      <c r="H99" s="64"/>
+      <c r="I99" s="91"/>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100" s="7"/>
       <c r="B100" s="19"/>
-      <c r="C100" s="97"/>
-      <c r="D100" s="122" t="s">
-        <v>73</v>
+      <c r="C100" s="85"/>
+      <c r="D100" s="110" t="s">
+        <v>70</v>
       </c>
       <c r="E100" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="F100" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="G100" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H100" s="52"/>
-      <c r="I100" s="103"/>
+      <c r="F100" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="G100" s="111" t="s">
+        <v>96</v>
+      </c>
+      <c r="H100" s="112"/>
+      <c r="I100" s="91"/>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="7"/>
       <c r="B101" s="19"/>
-      <c r="C101" s="97"/>
-      <c r="D101" s="123"/>
-      <c r="E101" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="F101" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="G101" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H101" s="52"/>
-      <c r="I101" s="103"/>
+      <c r="C101" s="85"/>
+      <c r="D101" s="113"/>
+      <c r="E101" s="55"/>
+      <c r="F101" s="55"/>
+      <c r="G101" s="55"/>
+      <c r="H101" s="55"/>
+      <c r="I101" s="91"/>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="7"/>
       <c r="B102" s="19"/>
-      <c r="C102" s="97"/>
-      <c r="D102" s="123"/>
-      <c r="E102" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="F102" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="G102" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="H102" s="52"/>
-      <c r="I102" s="103"/>
+      <c r="C102" s="85"/>
+      <c r="D102" s="113"/>
+      <c r="E102" s="55"/>
+      <c r="F102" s="55"/>
+      <c r="G102" s="55"/>
+      <c r="H102" s="55"/>
+      <c r="I102" s="91"/>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="7"/>
       <c r="B103" s="19"/>
-      <c r="C103" s="97"/>
-      <c r="D103" s="123"/>
-      <c r="E103" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="F103" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="G103" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="H103" s="52"/>
-      <c r="I103" s="103"/>
+      <c r="C103" s="85"/>
+      <c r="D103" s="113"/>
+      <c r="E103" s="55"/>
+      <c r="F103" s="55"/>
+      <c r="G103" s="55"/>
+      <c r="H103" s="55"/>
+      <c r="I103" s="91"/>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="7"/>
       <c r="B104" s="19"/>
-      <c r="C104" s="97"/>
-      <c r="D104" s="124"/>
-      <c r="E104" s="125"/>
-      <c r="F104" s="125"/>
-      <c r="G104" s="125"/>
-      <c r="H104" s="126"/>
-      <c r="I104" s="103"/>
-    </row>
-    <row r="105" ht="14.25" spans="1:9">
-      <c r="A105" s="127"/>
-      <c r="B105" s="128"/>
-      <c r="C105" s="129"/>
-      <c r="D105" s="130"/>
-      <c r="E105" s="86"/>
-      <c r="F105" s="86"/>
-      <c r="G105" s="86"/>
-      <c r="H105" s="87"/>
-      <c r="I105" s="131"/>
+      <c r="C104" s="85"/>
+      <c r="D104" s="113"/>
+      <c r="E104" s="55"/>
+      <c r="F104" s="55"/>
+      <c r="G104" s="55"/>
+      <c r="H104" s="55"/>
+      <c r="I104" s="91"/>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="7"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="85"/>
+      <c r="D105" s="113"/>
+      <c r="E105" s="55"/>
+      <c r="F105" s="55"/>
+      <c r="G105" s="55"/>
+      <c r="H105" s="55"/>
+      <c r="I105" s="91"/>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="7"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="85"/>
+      <c r="D106" s="114"/>
+      <c r="E106" s="115"/>
+      <c r="F106" s="115"/>
+      <c r="G106" s="115"/>
+      <c r="H106" s="116"/>
+      <c r="I106" s="91"/>
+    </row>
+    <row r="107" ht="14.25" spans="1:9">
+      <c r="A107" s="117"/>
+      <c r="B107" s="118"/>
+      <c r="C107" s="119"/>
+      <c r="D107" s="120"/>
+      <c r="E107" s="77"/>
+      <c r="F107" s="77"/>
+      <c r="G107" s="77"/>
+      <c r="H107" s="78"/>
+      <c r="I107" s="121"/>
     </row>
   </sheetData>
-  <mergeCells count="93">
+  <mergeCells count="87">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
@@ -5305,20 +5223,18 @@
     <mergeCell ref="F31:H31"/>
     <mergeCell ref="E32:H32"/>
     <mergeCell ref="E33:H33"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E41:H41"/>
     <mergeCell ref="E43:H43"/>
     <mergeCell ref="E44:H44"/>
     <mergeCell ref="F45:H45"/>
     <mergeCell ref="F46:H46"/>
     <mergeCell ref="F47:H47"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="E51:H51"/>
+    <mergeCell ref="E52:H52"/>
     <mergeCell ref="E56:H56"/>
     <mergeCell ref="E57:H57"/>
     <mergeCell ref="E59:H59"/>
@@ -5346,27 +5262,23 @@
     <mergeCell ref="E83:H83"/>
     <mergeCell ref="E84:H84"/>
     <mergeCell ref="E85:H85"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="E87:H87"/>
+    <mergeCell ref="E88:H88"/>
+    <mergeCell ref="E89:H89"/>
+    <mergeCell ref="E92:H92"/>
     <mergeCell ref="F98:H98"/>
     <mergeCell ref="G100:H100"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="G102:H102"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="A1:A105"/>
-    <mergeCell ref="B3:B105"/>
+    <mergeCell ref="A1:A107"/>
+    <mergeCell ref="B3:B107"/>
     <mergeCell ref="C3:C53"/>
-    <mergeCell ref="C56:C105"/>
+    <mergeCell ref="C56:C107"/>
     <mergeCell ref="D7:D30"/>
     <mergeCell ref="D35:D38"/>
     <mergeCell ref="D49:D52"/>
     <mergeCell ref="D60:D81"/>
     <mergeCell ref="D86:D89"/>
-    <mergeCell ref="D100:D103"/>
-    <mergeCell ref="I3:I105"/>
+    <mergeCell ref="D100:D105"/>
+    <mergeCell ref="I3:I107"/>
     <mergeCell ref="D39:H40"/>
   </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>